<commit_message>
updated sample inputs for better function demos
</commit_message>
<xml_diff>
--- a/sample_inputs/demo_packing_list1.xlsx
+++ b/sample_inputs/demo_packing_list1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cliff\Desktop\Personal projects\Programming\Python\shipping-label-app\sample_inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cliff\Desktop\Personal projects\Programming\Python\sample_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884FB079-1F5D-4A4B-81E1-5510049371D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B262EE-A84C-4741-AF13-F7608D708E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34065" yWindow="8280" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33015" yWindow="2520" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Packing List - 10 634498 - GT00" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>Ship To Address</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>89109</t>
+  </si>
+  <si>
+    <t>Mountain</t>
+  </si>
+  <si>
+    <t>Creek</t>
   </si>
 </sst>
 </file>
@@ -478,8 +484,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -494,10 +504,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,7 +728,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="16" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5:I7"/>
+      <selection pane="bottomLeft" activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -822,7 +828,7 @@
     </row>
     <row r="5" spans="1:35" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="52" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="53"/>
@@ -834,7 +840,7 @@
       <c r="I5" s="53"/>
       <c r="J5" s="2"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="62" t="s">
+      <c r="L5" s="54" t="s">
         <v>26</v>
       </c>
       <c r="M5" s="53"/>
@@ -843,12 +849,12 @@
       <c r="P5" s="53"/>
       <c r="Q5" s="53"/>
       <c r="R5" s="53"/>
-      <c r="S5" s="60"/>
+      <c r="S5" s="55"/>
       <c r="T5" s="13"/>
     </row>
     <row r="6" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="56" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="53"/>
@@ -860,7 +866,7 @@
       <c r="I6" s="53"/>
       <c r="J6" s="2"/>
       <c r="K6" s="13"/>
-      <c r="L6" s="62" t="s">
+      <c r="L6" s="54" t="s">
         <v>27</v>
       </c>
       <c r="M6" s="53"/>
@@ -869,7 +875,7 @@
       <c r="P6" s="53"/>
       <c r="Q6" s="53"/>
       <c r="R6" s="53"/>
-      <c r="S6" s="60"/>
+      <c r="S6" s="55"/>
       <c r="T6" s="13"/>
       <c r="V6" s="15" t="s">
         <v>4</v>
@@ -877,7 +883,7 @@
     </row>
     <row r="7" spans="1:35" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="52" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="53"/>
@@ -889,7 +895,7 @@
       <c r="I7" s="53"/>
       <c r="J7" s="2"/>
       <c r="K7" s="13"/>
-      <c r="L7" s="62" t="s">
+      <c r="L7" s="54" t="s">
         <v>28</v>
       </c>
       <c r="M7" s="53"/>
@@ -898,7 +904,7 @@
       <c r="P7" s="53"/>
       <c r="Q7" s="53"/>
       <c r="R7" s="53"/>
-      <c r="S7" s="60"/>
+      <c r="S7" s="55"/>
       <c r="T7" s="13"/>
       <c r="V7" s="15" t="s">
         <v>5</v>
@@ -906,7 +912,7 @@
     </row>
     <row r="8" spans="1:35" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
-      <c r="B8" s="52"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="53"/>
       <c r="D8" s="53"/>
       <c r="E8" s="2"/>
@@ -968,11 +974,11 @@
       </c>
       <c r="I10" s="2"/>
       <c r="K10" s="20"/>
-      <c r="L10" s="57"/>
+      <c r="L10" s="61"/>
       <c r="M10" s="53"/>
       <c r="N10" s="53"/>
       <c r="O10" s="53"/>
-      <c r="Q10" s="58"/>
+      <c r="Q10" s="62"/>
       <c r="R10" s="53"/>
       <c r="S10" s="17"/>
       <c r="T10" s="3"/>
@@ -989,11 +995,11 @@
       <c r="I11" s="2"/>
       <c r="J11" s="19"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="57"/>
+      <c r="L11" s="61"/>
       <c r="M11" s="53"/>
       <c r="N11" s="53"/>
       <c r="O11" s="53"/>
-      <c r="Q11" s="58"/>
+      <c r="Q11" s="62"/>
       <c r="R11" s="53"/>
       <c r="S11" s="17"/>
       <c r="T11" s="3"/>
@@ -1012,11 +1018,11 @@
       <c r="I12" s="2"/>
       <c r="J12" s="19"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="57"/>
+      <c r="L12" s="61"/>
       <c r="M12" s="53"/>
       <c r="N12" s="53"/>
       <c r="O12" s="53"/>
-      <c r="Q12" s="58"/>
+      <c r="Q12" s="62"/>
       <c r="R12" s="53"/>
       <c r="S12" s="17"/>
       <c r="T12" s="3"/>
@@ -1045,7 +1051,7 @@
         <f>IF(RIGHT(C16,LEN("(in)"))="(in)","Cubic Feet:","Cubic Meters")</f>
         <v>Cubic Feet:</v>
       </c>
-      <c r="C14" s="54">
+      <c r="C14" s="58">
         <f t="array" ref="C14">IF(RIGHT(C16,LEN("(in)"))="(in)",SUM((C17:C994*E17:E994*G17:G994)/1728),(SUM((C17:C994*E17:E994*G17:G994)/1728)*0.0283168))</f>
         <v>14.259259259259258</v>
       </c>
@@ -1065,7 +1071,7 @@
       <c r="L14" s="19"/>
       <c r="M14" s="19"/>
       <c r="N14" s="19"/>
-      <c r="P14" s="59" t="s">
+      <c r="P14" s="63" t="s">
         <v>11</v>
       </c>
       <c r="Q14" s="53"/>
@@ -1100,13 +1106,13 @@
         <f>"Carton # of "&amp;COUNT(B17:B22)</f>
         <v>Carton # of 5</v>
       </c>
-      <c r="C16" s="55" t="s">
+      <c r="C16" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
       <c r="H16" s="31" t="str">
         <f>IF(RIGHT(C16,LEN("(in)"))="(in)","Weight (lbs)","Weight KGS")</f>
         <v>Weight (lbs)</v>
@@ -1185,10 +1191,10 @@
         <v>41.2</v>
       </c>
       <c r="I17" s="39">
-        <v>673</v>
+        <v>438</v>
       </c>
       <c r="J17" s="41" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="K17" s="42"/>
       <c r="L17" s="42"/>
@@ -1275,10 +1281,10 @@
         <v>44.4</v>
       </c>
       <c r="I19" s="39">
-        <v>673</v>
+        <v>213</v>
       </c>
       <c r="J19" s="41" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="K19" s="42"/>
       <c r="L19" s="42"/>
@@ -1898,12 +1904,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="L5:S5"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="L6:S6"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="L7:S7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C16:G16"/>
@@ -1914,6 +1914,12 @@
     <mergeCell ref="L12:O12"/>
     <mergeCell ref="Q12:R12"/>
     <mergeCell ref="P14:R14"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="L5:S5"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="L6:S6"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="L7:S7"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C16" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>